<commit_message>
python scripts and data for winter all morph
</commit_message>
<xml_diff>
--- a/avbernat_working_on/allmorphology_scripts_and_data/update on 04.20.2020/morph_to_cp-winter2020.xlsx
+++ b/avbernat_working_on/allmorphology_scripts_and_data/update on 04.20.2020/morph_to_cp-winter2020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/allmorph/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E6C417-04B5-5C40-9A45-9817FCABBFB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3428BAA8-BF4E-2D41-8CB3-BC2E895CCC1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="460" windowWidth="16600" windowHeight="16240" xr2:uid="{119300D4-B62B-7749-95EB-18D5D862CFD8}"/>
   </bookViews>
@@ -620,7 +620,7 @@
   <dimension ref="A1:T335"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1136,10 +1136,10 @@
         <v>27</v>
       </c>
       <c r="E13" s="2">
+        <v>8.7899999999999991</v>
+      </c>
+      <c r="F13" s="2">
         <v>3.86</v>
-      </c>
-      <c r="F13" s="2">
-        <v>8.7899999999999991</v>
       </c>
       <c r="G13" s="2">
         <v>10.07</v>

</xml_diff>